<commit_message>
files from simulation in portimao
</commit_message>
<xml_diff>
--- a/+Model/LMP2_OS.xlsx
+++ b/+Model/LMP2_OS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\LaptimeSimOCP\+Model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6692039-52EA-4CC1-9AF7-B1BEBD34877E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E91CB05B-B183-4FCB-9B6A-A25E5864AE27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="9" xr2:uid="{C9770ACA-89D6-4C25-A406-8CFD34B6BEB6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="2" activeTab="7" xr2:uid="{C9770ACA-89D6-4C25-A406-8CFD34B6BEB6}"/>
   </bookViews>
   <sheets>
     <sheet name="MassInertia" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="46">
   <si>
     <t>setup</t>
   </si>
@@ -176,6 +176,12 @@
   </si>
   <si>
     <t>maximum_torque</t>
+  </si>
+  <si>
+    <t>gear_ratio</t>
+  </si>
+  <si>
+    <t>GearRatio.xlsx</t>
   </si>
 </sst>
 </file>
@@ -531,15 +537,15 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -574,7 +580,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -617,21 +623,22 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{438D574D-38FE-45DB-9CEC-921C97E214E2}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>25</v>
       </c>
@@ -644,10 +651,13 @@
       <c r="D1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>3.1</v>
+        <v>3.5</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -657,6 +667,9 @@
       </c>
       <c r="D2" t="s">
         <v>29</v>
+      </c>
+      <c r="E2" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -673,13 +686,13 @@
       <selection activeCell="A3" sqref="A3:C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -690,7 +703,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>3.0049999999999999</v>
       </c>
@@ -714,9 +727,9 @@
       <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>35</v>
       </c>
@@ -745,7 +758,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
@@ -785,12 +798,12 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -807,7 +820,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1.0029999999999999</v>
       </c>
@@ -838,16 +851,16 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>0.51</v>
+        <v>0.56000000000000005</v>
       </c>
     </row>
   </sheetData>
@@ -863,12 +876,12 @@
       <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -879,7 +892,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2E-3</v>
       </c>
@@ -903,12 +916,12 @@
       <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -919,7 +932,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2E-3</v>
       </c>
@@ -939,16 +952,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E935BBC8-6905-40C4-93AA-35113AE6796F}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>24</v>
       </c>
@@ -956,7 +969,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2">
         <f>0.7</f>
         <v>0.7</v>
@@ -965,13 +978,13 @@
         <v>6000</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B3" s="1"/>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B4" s="1"/>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B5" s="1"/>
     </row>
   </sheetData>
@@ -988,9 +1001,9 @@
       <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>32</v>
       </c>
@@ -998,7 +1011,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>50</v>
       </c>

</xml_diff>

<commit_message>
Gear change implementation in getWheelTorques3 function and results from portimao
</commit_message>
<xml_diff>
--- a/+Model/LMP2_OS.xlsx
+++ b/+Model/LMP2_OS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\LaptimeSimOCP\+Model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6692039-52EA-4CC1-9AF7-B1BEBD34877E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E91CB05B-B183-4FCB-9B6A-A25E5864AE27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="9" xr2:uid="{C9770ACA-89D6-4C25-A406-8CFD34B6BEB6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="2" activeTab="7" xr2:uid="{C9770ACA-89D6-4C25-A406-8CFD34B6BEB6}"/>
   </bookViews>
   <sheets>
     <sheet name="MassInertia" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="46">
   <si>
     <t>setup</t>
   </si>
@@ -176,6 +176,12 @@
   </si>
   <si>
     <t>maximum_torque</t>
+  </si>
+  <si>
+    <t>gear_ratio</t>
+  </si>
+  <si>
+    <t>GearRatio.xlsx</t>
   </si>
 </sst>
 </file>
@@ -531,15 +537,15 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -574,7 +580,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -617,21 +623,22 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{438D574D-38FE-45DB-9CEC-921C97E214E2}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>25</v>
       </c>
@@ -644,10 +651,13 @@
       <c r="D1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>3.1</v>
+        <v>3.5</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -657,6 +667,9 @@
       </c>
       <c r="D2" t="s">
         <v>29</v>
+      </c>
+      <c r="E2" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -673,13 +686,13 @@
       <selection activeCell="A3" sqref="A3:C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -690,7 +703,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>3.0049999999999999</v>
       </c>
@@ -714,9 +727,9 @@
       <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>35</v>
       </c>
@@ -745,7 +758,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
@@ -785,12 +798,12 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -807,7 +820,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1.0029999999999999</v>
       </c>
@@ -838,16 +851,16 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>0.51</v>
+        <v>0.56000000000000005</v>
       </c>
     </row>
   </sheetData>
@@ -863,12 +876,12 @@
       <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -879,7 +892,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2E-3</v>
       </c>
@@ -903,12 +916,12 @@
       <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -919,7 +932,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2E-3</v>
       </c>
@@ -939,16 +952,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E935BBC8-6905-40C4-93AA-35113AE6796F}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>24</v>
       </c>
@@ -956,7 +969,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2">
         <f>0.7</f>
         <v>0.7</v>
@@ -965,13 +978,13 @@
         <v>6000</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B3" s="1"/>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B4" s="1"/>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B5" s="1"/>
     </row>
   </sheetData>
@@ -988,9 +1001,9 @@
       <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>32</v>
       </c>
@@ -998,7 +1011,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>50</v>
       </c>

</xml_diff>

<commit_message>
Implemented track generation from GPS data for bahrein
</commit_message>
<xml_diff>
--- a/+Model/LMP2_OS.xlsx
+++ b/+Model/LMP2_OS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\LaptimeSimOCP\+Model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6692039-52EA-4CC1-9AF7-B1BEBD34877E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CDC3E16-A6A3-48B3-9C0F-E2DB3101301B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="9" xr2:uid="{C9770ACA-89D6-4C25-A406-8CFD34B6BEB6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{C9770ACA-89D6-4C25-A406-8CFD34B6BEB6}"/>
   </bookViews>
   <sheets>
     <sheet name="MassInertia" sheetId="1" r:id="rId1"/>
@@ -530,16 +530,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E820AE81-6940-42C1-9794-755A660CF3D0}">
   <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -574,7 +574,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -582,10 +582,10 @@
         <v>17</v>
       </c>
       <c r="C2">
-        <v>965</v>
+        <v>1050</v>
       </c>
       <c r="D2">
-        <v>1400</v>
+        <v>1750</v>
       </c>
       <c r="E2">
         <v>3.7050000000000001</v>
@@ -619,19 +619,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{438D574D-38FE-45DB-9CEC-921C97E214E2}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>25</v>
       </c>
@@ -645,15 +645,15 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>3.1</v>
+        <v>2.9</v>
       </c>
       <c r="B2">
         <v>0</v>
       </c>
       <c r="C2">
-        <v>550</v>
+        <v>500</v>
       </c>
       <c r="D2" t="s">
         <v>29</v>
@@ -673,13 +673,13 @@
       <selection activeCell="A3" sqref="A3:C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -690,7 +690,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>3.0049999999999999</v>
       </c>
@@ -714,9 +714,9 @@
       <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>35</v>
       </c>
@@ -745,7 +745,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
@@ -785,12 +785,12 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -807,12 +807,12 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1.0029999999999999</v>
       </c>
       <c r="B2">
-        <v>5</v>
+        <v>4.5</v>
       </c>
       <c r="C2">
         <v>1.2250000000000001</v>
@@ -838,16 +838,16 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>0.51</v>
+        <v>0.55000000000000004</v>
       </c>
     </row>
   </sheetData>
@@ -863,12 +863,12 @@
       <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -879,7 +879,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2E-3</v>
       </c>
@@ -900,15 +900,15 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -919,7 +919,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2E-3</v>
       </c>
@@ -943,12 +943,12 @@
       <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>24</v>
       </c>
@@ -956,7 +956,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2">
         <f>0.7</f>
         <v>0.7</v>
@@ -965,13 +965,13 @@
         <v>6000</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B3" s="1"/>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B4" s="1"/>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B5" s="1"/>
     </row>
   </sheetData>
@@ -988,9 +988,9 @@
       <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>32</v>
       </c>
@@ -998,7 +998,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>50</v>
       </c>

</xml_diff>